<commit_message>
Found our best policy
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>alpha</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>10 million eps</t>
+  </si>
+  <si>
+    <t>evaluation</t>
+  </si>
+  <si>
+    <t>sucks</t>
   </si>
 </sst>
 </file>
@@ -362,15 +368,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,7 +387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1E-3</v>
       </c>
@@ -392,7 +398,7 @@
         <v>7.1665000000000006E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1E-3</v>
       </c>
@@ -402,8 +408,14 @@
       <c r="C3">
         <v>7.2551000000000004E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3">
+        <v>-4.8906999999999999E-2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>1E-3</v>
       </c>
@@ -414,7 +426,7 @@
         <v>6.9379999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>1E-3</v>
       </c>
@@ -425,7 +437,7 @@
         <v>7.0818000000000006E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>1E-3</v>
       </c>
@@ -436,7 +448,7 @@
         <v>6.8106E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>1E-3</v>
       </c>
@@ -447,7 +459,7 @@
         <v>7.0319000000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>1E-3</v>
       </c>
@@ -458,7 +470,7 @@
         <v>6.8298999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -469,7 +481,7 @@
         <v>5.7657E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -480,7 +492,7 @@
         <v>5.8284000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -491,7 +503,7 @@
         <v>5.4349000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -502,7 +514,7 @@
         <v>5.4670999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>0.01</v>
       </c>
@@ -513,7 +525,7 @@
         <v>5.4088999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -523,11 +535,8 @@
       <c r="C14">
         <v>5.1166000000000003E-2</v>
       </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+    </row>
+    <row r="15" spans="1:7">
       <c r="C15">
         <v>4.6985499999999999E-2</v>
       </c>
@@ -535,9 +544,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="4:4">
-      <c r="D18">
-        <v>-4.8906999999999999E-2</v>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="B16">
+        <v>2E-3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="B17">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C17">
+        <v>5.5397000000000002E-2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>